<commit_message>
The new board is ready for DPTs and further tests. The current measurement specs are not tested for now. The laboratory is ridiculously cold.
</commit_message>
<xml_diff>
--- a/Project/3501/Furkan/IMMD Production/Test sonuçları/Kart 1 sonuçlar.xlsx
+++ b/Project/3501/Furkan/IMMD Production/Test sonuçları/Kart 1 sonuçlar.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="193">
   <si>
     <t>Test Edilecek Birim</t>
   </si>
@@ -684,7 +684,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -693,6 +693,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -769,7 +770,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3260,8 +3260,8 @@
   </sheetPr>
   <dimension ref="A1:G109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G40" sqref="G40"/>
+    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J104" sqref="J104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4622,7 +4622,7 @@
         <v>-10</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="4">
         <v>67</v>
       </c>
@@ -4642,7 +4642,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="4">
         <v>68</v>
       </c>
@@ -4662,7 +4662,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="4">
         <v>69</v>
       </c>
@@ -4682,7 +4682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="4">
         <v>70</v>
       </c>
@@ -4702,7 +4702,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="4">
         <v>71</v>
       </c>
@@ -4722,7 +4722,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="4">
         <v>72</v>
       </c>
@@ -4742,7 +4742,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="4">
         <v>73</v>
       </c>
@@ -4762,7 +4762,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="4">
         <v>74</v>
       </c>
@@ -4782,7 +4782,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="5">
         <v>75</v>
       </c>
@@ -4801,8 +4801,11 @@
       <c r="F73" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G73" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="5">
         <v>76</v>
       </c>
@@ -4821,8 +4824,11 @@
       <c r="F74" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G74" s="8">
+        <v>9.3000000000000007</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="5">
         <v>77</v>
       </c>
@@ -4841,8 +4847,11 @@
       <c r="F75" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G75" s="8">
+        <v>5.9130000000000003</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="5">
         <v>78</v>
       </c>
@@ -4861,8 +4870,11 @@
       <c r="F76" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G76" s="8">
+        <v>-3.383</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="4">
         <v>79</v>
       </c>
@@ -4881,8 +4893,11 @@
       <c r="F77" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G77" s="8" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="4">
         <v>80</v>
       </c>
@@ -4901,8 +4916,11 @@
       <c r="F78" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G78" s="8">
+        <v>9.3000000000000007</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="4">
         <v>81</v>
       </c>
@@ -4921,8 +4939,11 @@
       <c r="F79" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G79" s="8">
+        <v>5.915</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="4">
         <v>82</v>
       </c>
@@ -4941,8 +4962,11 @@
       <c r="F80" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G80" s="8">
+        <v>-3.3849999999999998</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="5">
         <v>83</v>
       </c>
@@ -4961,8 +4985,11 @@
       <c r="F81" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G81" s="8" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="5">
         <v>84</v>
       </c>
@@ -4981,8 +5008,11 @@
       <c r="F82" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G82" s="8" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="5">
         <v>85</v>
       </c>
@@ -5001,8 +5031,11 @@
       <c r="F83" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G83" s="8" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="4">
         <v>86</v>
       </c>
@@ -5021,8 +5054,11 @@
       <c r="F84" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G84" s="8" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="4">
         <v>87</v>
       </c>
@@ -5041,8 +5077,11 @@
       <c r="F85" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G85" s="8">
+        <v>9.3000000000000007</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="4">
         <v>88</v>
       </c>
@@ -5061,8 +5100,11 @@
       <c r="F86" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G86" s="8">
+        <v>5.9260000000000002</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="4">
         <v>89</v>
       </c>
@@ -5081,8 +5123,11 @@
       <c r="F87" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G87" s="8">
+        <v>-3.3690000000000002</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="5">
         <v>90</v>
       </c>
@@ -5101,8 +5146,11 @@
       <c r="F88" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G88" s="8" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="5">
         <v>91</v>
       </c>
@@ -5121,8 +5169,11 @@
       <c r="F89" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G89" s="8">
+        <v>9.32</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="5">
         <v>92</v>
       </c>
@@ -5141,8 +5192,11 @@
       <c r="F90" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G90" s="8">
+        <v>5.93</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="5">
         <v>93</v>
       </c>
@@ -5161,8 +5215,11 @@
       <c r="F91" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G91" s="8">
+        <v>-3.3849999999999998</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="4">
         <v>94</v>
       </c>
@@ -5181,8 +5238,11 @@
       <c r="F92" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G92" s="8" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="4">
         <v>95</v>
       </c>
@@ -5201,8 +5261,11 @@
       <c r="F93" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G93" s="8" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="4">
         <v>96</v>
       </c>
@@ -5221,8 +5284,11 @@
       <c r="F94" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G94" s="8" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="5">
         <v>97</v>
       </c>
@@ -5241,8 +5307,11 @@
       <c r="F95" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G95" s="8" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" s="5">
         <v>98</v>
       </c>
@@ -5261,8 +5330,11 @@
       <c r="F96" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G96" s="8">
+        <v>9.3000000000000007</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="5">
         <v>99</v>
       </c>
@@ -5281,8 +5353,11 @@
       <c r="F97" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G97" s="8">
+        <v>5.9340000000000002</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" s="5">
         <v>100</v>
       </c>
@@ -5301,8 +5376,11 @@
       <c r="F98" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G98" s="8">
+        <v>-3.3679999999999999</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" s="4">
         <v>101</v>
       </c>
@@ -5321,8 +5399,11 @@
       <c r="F99" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G99" s="8" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" s="4">
         <v>102</v>
       </c>
@@ -5341,8 +5422,11 @@
       <c r="F100" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G100" s="8">
+        <v>9.32</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" s="4">
         <v>103</v>
       </c>
@@ -5361,8 +5445,11 @@
       <c r="F101" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G101" s="8">
+        <v>5.9320000000000004</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" s="4">
         <v>104</v>
       </c>
@@ -5381,8 +5468,11 @@
       <c r="F102" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G102" s="8">
+        <v>-3.387</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" s="5">
         <v>105</v>
       </c>
@@ -5401,8 +5491,11 @@
       <c r="F103" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G103" s="8" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" s="5">
         <v>106</v>
       </c>
@@ -5421,8 +5514,11 @@
       <c r="F104" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G104" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" s="5">
         <v>107</v>
       </c>
@@ -5441,8 +5537,11 @@
       <c r="F105" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G105" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" s="4">
         <v>108</v>
       </c>
@@ -5462,7 +5561,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" s="4">
         <v>109</v>
       </c>
@@ -5482,7 +5581,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" s="4">
         <v>110</v>
       </c>
@@ -5502,7 +5601,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B109" t="s">
         <v>191</v>
       </c>

</xml_diff>